<commit_message>
Full Dashboard After Some Changes
</commit_message>
<xml_diff>
--- a/Node_relationship.xlsx
+++ b/Node_relationship.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nandhu\comeai\Result_Share\Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C14A3F-4205-4518-8A90-BB54B815518E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A090B20F-9A2F-4F72-9995-E4E1C0CCDC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{87162CFC-B4E0-45F1-A01A-41825A97D9AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{87162CFC-B4E0-45F1-A01A-41825A97D9AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$140</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$139</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="117">
   <si>
     <t>F2_1</t>
   </si>
@@ -763,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A99ED6B7-327B-491C-9CB5-D727B291EEBF}">
-  <dimension ref="A1:B140"/>
+  <dimension ref="A1:B139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -872,7 +872,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -880,23 +880,23 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -904,15 +904,15 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -920,7 +920,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -928,15 +928,15 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
@@ -944,15 +944,15 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
@@ -960,15 +960,15 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -976,15 +976,15 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B27" t="s">
         <v>11</v>
@@ -992,10 +992,10 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -1008,15 +1008,15 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
         <v>13</v>
@@ -1024,15 +1024,15 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B33" t="s">
         <v>14</v>
@@ -1040,10 +1040,10 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -1064,15 +1064,15 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B37" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B38" t="s">
         <v>16</v>
@@ -1080,15 +1080,15 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B40" t="s">
         <v>17</v>
@@ -1096,15 +1096,15 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B41" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B42" t="s">
         <v>18</v>
@@ -1112,7 +1112,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B43" t="s">
         <v>18</v>
@@ -1120,10 +1120,10 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B44" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -1136,15 +1136,15 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B46" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B47" t="s">
         <v>20</v>
@@ -1152,15 +1152,15 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B49" t="s">
         <v>21</v>
@@ -1168,7 +1168,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B50" t="s">
         <v>21</v>
@@ -1176,15 +1176,15 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B52" t="s">
         <v>22</v>
@@ -1192,7 +1192,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B53" t="s">
         <v>22</v>
@@ -1200,15 +1200,15 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B54" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B55" t="s">
         <v>23</v>
@@ -1216,15 +1216,15 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B56" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B57" t="s">
         <v>24</v>
@@ -1232,15 +1232,15 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B59" t="s">
         <v>25</v>
@@ -1248,15 +1248,15 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B60" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B61" t="s">
         <v>26</v>
@@ -1264,15 +1264,15 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B62" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B63" t="s">
         <v>27</v>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B64" t="s">
         <v>27</v>
@@ -1288,15 +1288,15 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="B65" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B66" t="s">
         <v>28</v>
@@ -1304,15 +1304,15 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B67" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B68" t="s">
         <v>29</v>
@@ -1320,15 +1320,15 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B69" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B70" t="s">
         <v>30</v>
@@ -1336,7 +1336,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B71" t="s">
         <v>30</v>
@@ -1344,15 +1344,15 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B72" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B73" t="s">
         <v>31</v>
@@ -1368,15 +1368,15 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="B75" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B76" t="s">
         <v>32</v>
@@ -1384,15 +1384,15 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B77" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B78" t="s">
         <v>33</v>
@@ -1400,15 +1400,15 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
+        <v>96</v>
+      </c>
+      <c r="B79" t="s">
         <v>34</v>
-      </c>
-      <c r="B79" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B80" t="s">
         <v>34</v>
@@ -1416,7 +1416,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B81" t="s">
         <v>34</v>
@@ -1424,15 +1424,15 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>88</v>
+        <v>32</v>
       </c>
       <c r="B82" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B83" t="s">
         <v>35</v>
@@ -1440,7 +1440,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B84" t="s">
         <v>35</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="B85" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -1464,15 +1464,15 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B87" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B88" t="s">
         <v>37</v>
@@ -1480,7 +1480,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B89" t="s">
         <v>37</v>
@@ -1488,15 +1488,15 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B90" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B91" t="s">
         <v>38</v>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B92" t="s">
         <v>38</v>
@@ -1515,12 +1515,12 @@
         <v>97</v>
       </c>
       <c r="B93" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B94" t="s">
         <v>39</v>
@@ -1528,7 +1528,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B95" t="s">
         <v>39</v>
@@ -1536,15 +1536,15 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B96" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B97" t="s">
         <v>40</v>
@@ -1552,15 +1552,15 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B98" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B99" t="s">
         <v>41</v>
@@ -1568,7 +1568,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B100" t="s">
         <v>41</v>
@@ -1576,15 +1576,15 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B101" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B102" t="s">
         <v>42</v>
@@ -1592,15 +1592,15 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>105</v>
+        <v>37</v>
       </c>
       <c r="B103" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B104" t="s">
         <v>43</v>
@@ -1608,7 +1608,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B105" t="s">
         <v>43</v>
@@ -1616,15 +1616,15 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B106" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B107" t="s">
         <v>44</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B108" t="s">
         <v>44</v>
@@ -1640,15 +1640,15 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B109" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B110" t="s">
         <v>45</v>
@@ -1656,15 +1656,15 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B111" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B112" t="s">
         <v>46</v>
@@ -1672,15 +1672,15 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="B113" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B114" t="s">
         <v>47</v>
@@ -1688,15 +1688,15 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B115" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B116" t="s">
         <v>48</v>
@@ -1704,15 +1704,15 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B117" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B118" t="s">
         <v>49</v>
@@ -1720,7 +1720,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B119" t="s">
         <v>49</v>
@@ -1728,15 +1728,15 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B120" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B121" t="s">
         <v>50</v>
@@ -1744,15 +1744,15 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B122" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B123" t="s">
         <v>51</v>
@@ -1760,7 +1760,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B124" t="s">
         <v>51</v>
@@ -1768,15 +1768,15 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>106</v>
+        <v>47</v>
       </c>
       <c r="B125" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B126" t="s">
         <v>52</v>
@@ -1784,15 +1784,15 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B127" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B128" t="s">
         <v>53</v>
@@ -1800,7 +1800,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B129" t="s">
         <v>53</v>
@@ -1808,15 +1808,15 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B130" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B131" t="s">
         <v>54</v>
@@ -1824,15 +1824,15 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="B132" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B133" t="s">
         <v>55</v>
@@ -1840,7 +1840,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B134" t="s">
         <v>55</v>
@@ -1848,7 +1848,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B135" t="s">
         <v>55</v>
@@ -1856,15 +1856,15 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>35</v>
+        <v>115</v>
       </c>
       <c r="B136" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="B137" t="s">
         <v>56</v>
@@ -1872,7 +1872,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B138" t="s">
         <v>56</v>
@@ -1880,17 +1880,9 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="B139" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
-        <v>116</v>
-      </c>
-      <c r="B140" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
After fixing Node relations
</commit_message>
<xml_diff>
--- a/Node_relationship.xlsx
+++ b/Node_relationship.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nandhu\comeai\Result_Share\Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A090B20F-9A2F-4F72-9995-E4E1C0CCDC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B83C25-6C1F-4384-9647-54BDBF02C7C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{87162CFC-B4E0-45F1-A01A-41825A97D9AF}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="193">
   <si>
     <t>F2_1</t>
   </si>
@@ -221,176 +221,535 @@
     <t>child</t>
   </si>
   <si>
-    <t>FI_1</t>
-  </si>
-  <si>
-    <t>FI_2</t>
-  </si>
-  <si>
-    <t>FI_5</t>
-  </si>
-  <si>
-    <t>FI_4</t>
-  </si>
-  <si>
-    <t>F1_1</t>
-  </si>
-  <si>
-    <t>FI_3</t>
-  </si>
-  <si>
-    <t>FI_6</t>
-  </si>
-  <si>
-    <t>FI_7</t>
-  </si>
-  <si>
-    <t>FI_8</t>
-  </si>
-  <si>
-    <t>FI_9</t>
-  </si>
-  <si>
-    <t>I1_1</t>
-  </si>
-  <si>
-    <t>I1_4</t>
-  </si>
-  <si>
-    <t>I1_2</t>
-  </si>
-  <si>
-    <t>I1_5</t>
-  </si>
-  <si>
-    <t>I1_3</t>
-  </si>
-  <si>
-    <t>I1_6</t>
-  </si>
-  <si>
-    <t>I1_8</t>
-  </si>
-  <si>
-    <t>I1_9</t>
-  </si>
-  <si>
-    <t>I1_7</t>
-  </si>
-  <si>
-    <t>H1_1</t>
-  </si>
-  <si>
-    <t>H1_2</t>
-  </si>
-  <si>
-    <t>H1_4</t>
-  </si>
-  <si>
-    <t>H1_3</t>
-  </si>
-  <si>
-    <t>H1_5</t>
-  </si>
-  <si>
-    <t>H1_7</t>
-  </si>
-  <si>
-    <t>H1_6</t>
-  </si>
-  <si>
-    <t>H1_9</t>
-  </si>
-  <si>
-    <t>H1_8</t>
-  </si>
-  <si>
-    <t>E1_1</t>
-  </si>
-  <si>
-    <t>E1_2</t>
-  </si>
-  <si>
-    <t>E1_5</t>
-  </si>
-  <si>
-    <t>E1_4</t>
-  </si>
-  <si>
-    <t>E1_7</t>
-  </si>
-  <si>
-    <t>E1_9</t>
-  </si>
-  <si>
-    <t>E1_6</t>
-  </si>
-  <si>
-    <t>E1_3</t>
-  </si>
-  <si>
-    <t>E1_8</t>
-  </si>
-  <si>
-    <t>C1_1</t>
-  </si>
-  <si>
-    <t>C1_2</t>
-  </si>
-  <si>
-    <t>C1_3</t>
-  </si>
-  <si>
-    <t>C1_4</t>
-  </si>
-  <si>
-    <t>C1_7</t>
-  </si>
-  <si>
-    <t>C1_8</t>
-  </si>
-  <si>
-    <t>C1_9</t>
-  </si>
-  <si>
-    <t>C1_5</t>
-  </si>
-  <si>
-    <t>C1_6</t>
-  </si>
-  <si>
-    <t>G1_1</t>
-  </si>
-  <si>
-    <t>G1_7</t>
-  </si>
-  <si>
-    <t>G1_8</t>
-  </si>
-  <si>
-    <t>G1_5</t>
-  </si>
-  <si>
-    <t>G1_3</t>
-  </si>
-  <si>
-    <t>G1_6</t>
-  </si>
-  <si>
-    <t>G1_2</t>
-  </si>
-  <si>
-    <t>G1_4</t>
-  </si>
-  <si>
-    <t>G1_9</t>
-  </si>
-  <si>
     <t xml:space="preserve">W_1
 </t>
   </si>
   <si>
     <t xml:space="preserve">W_2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI_2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI_5
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI_4
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1_13
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F2_2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI_3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI_7
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI_10
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI_12
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI_9
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI_11
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F2_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F2_3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F2_4
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F2_5
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F2_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F3_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F3_2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I1_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I1_4
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I1_2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I1_5
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I1_3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I1_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I1_10
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I1_11
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I1_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I1_9
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I1_7
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I1_12
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H1_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H1_12
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H1_13
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H1_2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H1_4
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H1_3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H1_5
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H1_7
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H1_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H1_10
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H1_11
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H1_9
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H1_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2_4
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2_2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2_5
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2_3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I3_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I3_2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2_2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2_3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2_4
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2_5
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H3_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H3_2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H3_3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1_2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1_5
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1_4
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1_7
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1_9
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1_3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1_10
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1_13
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E2_2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E2_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E2_3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E2_5
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1_15
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E3_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E3_2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E3_3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1_12
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1_11
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1_2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1_10
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1_3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1_12
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1_4
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1_11
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1_7
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1_9
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1_5
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2_2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2_3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2_4
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2_5
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3_2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E2_4
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E2_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G1_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G1_7
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G1_8
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G1_11
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G1_5
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G1_3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G1_6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G1_2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G1_12
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G1_4
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G1_9
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G1_10
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G2_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G2_2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G2_3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G2_4
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G2_5
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G3_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G3_2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F4_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H4_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I4_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E4_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C4_1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G4_1
 </t>
   </si>
 </sst>
@@ -763,10 +1122,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A99ED6B7-327B-491C-9CB5-D727B291EEBF}">
-  <dimension ref="A1:B139"/>
+  <dimension ref="A1:B140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,7 +1143,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -792,7 +1151,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -800,7 +1159,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -808,7 +1167,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -816,7 +1175,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -824,7 +1183,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -832,7 +1191,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -840,7 +1199,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -848,7 +1207,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -856,7 +1215,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -864,7 +1223,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -872,7 +1231,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -880,23 +1239,23 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -904,15 +1263,15 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -920,7 +1279,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -928,15 +1287,15 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
@@ -944,15 +1303,15 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
@@ -960,15 +1319,15 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -976,15 +1335,15 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="B27" t="s">
         <v>11</v>
@@ -992,15 +1351,15 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="B29" t="s">
         <v>12</v>
@@ -1008,15 +1367,15 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="B31" t="s">
         <v>13</v>
@@ -1024,15 +1383,15 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="B33" t="s">
         <v>14</v>
@@ -1040,15 +1399,15 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="B35" t="s">
         <v>15</v>
@@ -1056,7 +1415,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="B36" t="s">
         <v>15</v>
@@ -1064,15 +1423,15 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s">
         <v>16</v>
@@ -1080,15 +1439,15 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="B39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="B40" t="s">
         <v>17</v>
@@ -1096,15 +1455,15 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="B42" t="s">
         <v>18</v>
@@ -1112,7 +1471,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="B43" t="s">
         <v>18</v>
@@ -1120,15 +1479,15 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="B44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="B45" t="s">
         <v>19</v>
@@ -1136,15 +1495,15 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="B46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="B47" t="s">
         <v>20</v>
@@ -1152,15 +1511,15 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>9</v>
+        <v>107</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
       <c r="B49" t="s">
         <v>21</v>
@@ -1168,7 +1527,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="B50" t="s">
         <v>21</v>
@@ -1176,15 +1535,15 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="B51" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="B52" t="s">
         <v>22</v>
@@ -1192,7 +1551,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="B53" t="s">
         <v>22</v>
@@ -1200,15 +1559,15 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="B54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
       <c r="B55" t="s">
         <v>23</v>
@@ -1216,15 +1575,15 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>15</v>
+        <v>115</v>
       </c>
       <c r="B56" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="B57" t="s">
         <v>24</v>
@@ -1232,15 +1591,15 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>17</v>
+        <v>117</v>
       </c>
       <c r="B58" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>18</v>
+        <v>118</v>
       </c>
       <c r="B59" t="s">
         <v>25</v>
@@ -1248,15 +1607,15 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>19</v>
+        <v>119</v>
       </c>
       <c r="B60" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="B61" t="s">
         <v>26</v>
@@ -1264,15 +1623,15 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>24</v>
+        <v>121</v>
       </c>
       <c r="B62" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>25</v>
+        <v>122</v>
       </c>
       <c r="B63" t="s">
         <v>27</v>
@@ -1280,7 +1639,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>26</v>
+        <v>123</v>
       </c>
       <c r="B64" t="s">
         <v>27</v>
@@ -1288,15 +1647,15 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>88</v>
+        <v>124</v>
       </c>
       <c r="B65" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
       <c r="B66" t="s">
         <v>28</v>
@@ -1304,15 +1663,15 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="B67" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="B68" t="s">
         <v>29</v>
@@ -1320,15 +1679,15 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="B69" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="B70" t="s">
         <v>30</v>
@@ -1336,7 +1695,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
       <c r="B71" t="s">
         <v>30</v>
@@ -1344,15 +1703,15 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="B72" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>88</v>
+        <v>132</v>
       </c>
       <c r="B73" t="s">
         <v>31</v>
@@ -1360,7 +1719,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>88</v>
+        <v>133</v>
       </c>
       <c r="B74" t="s">
         <v>31</v>
@@ -1368,15 +1727,15 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>29</v>
+        <v>134</v>
       </c>
       <c r="B75" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>28</v>
+        <v>135</v>
       </c>
       <c r="B76" t="s">
         <v>32</v>
@@ -1384,15 +1743,15 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>30</v>
+        <v>136</v>
       </c>
       <c r="B77" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>34</v>
+        <v>137</v>
       </c>
       <c r="B78" t="s">
         <v>33</v>
@@ -1400,15 +1759,15 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="B79" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="B80" t="s">
         <v>34</v>
@@ -1416,7 +1775,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>88</v>
+        <v>131</v>
       </c>
       <c r="B81" t="s">
         <v>34</v>
@@ -1424,15 +1783,15 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>32</v>
+        <v>140</v>
       </c>
       <c r="B82" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>33</v>
+        <v>141</v>
       </c>
       <c r="B83" t="s">
         <v>35</v>
@@ -1440,7 +1799,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>46</v>
+        <v>142</v>
       </c>
       <c r="B84" t="s">
         <v>35</v>
@@ -1448,15 +1807,15 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>88</v>
+        <v>143</v>
       </c>
       <c r="B85" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>88</v>
+        <v>144</v>
       </c>
       <c r="B86" t="s">
         <v>36</v>
@@ -1464,15 +1823,15 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>97</v>
+        <v>145</v>
       </c>
       <c r="B87" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>98</v>
+        <v>146</v>
       </c>
       <c r="B88" t="s">
         <v>37</v>
@@ -1480,7 +1839,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>97</v>
+        <v>147</v>
       </c>
       <c r="B89" t="s">
         <v>37</v>
@@ -1488,15 +1847,15 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="B90" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>98</v>
+        <v>149</v>
       </c>
       <c r="B91" t="s">
         <v>38</v>
@@ -1504,7 +1863,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>97</v>
+        <v>147</v>
       </c>
       <c r="B92" t="s">
         <v>38</v>
@@ -1512,15 +1871,15 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>97</v>
+        <v>148</v>
       </c>
       <c r="B93" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="B94" t="s">
         <v>39</v>
@@ -1528,7 +1887,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>147</v>
       </c>
       <c r="B95" t="s">
         <v>39</v>
@@ -1536,15 +1895,15 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>100</v>
+        <v>148</v>
       </c>
       <c r="B96" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>97</v>
+        <v>151</v>
       </c>
       <c r="B97" t="s">
         <v>40</v>
@@ -1552,15 +1911,15 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>101</v>
+        <v>152</v>
       </c>
       <c r="B98" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
       <c r="B99" t="s">
         <v>41</v>
@@ -1568,7 +1927,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>103</v>
+        <v>154</v>
       </c>
       <c r="B100" t="s">
         <v>41</v>
@@ -1576,15 +1935,15 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>104</v>
+        <v>155</v>
       </c>
       <c r="B101" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>105</v>
+        <v>156</v>
       </c>
       <c r="B102" t="s">
         <v>42</v>
@@ -1592,15 +1951,15 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>37</v>
+        <v>157</v>
       </c>
       <c r="B103" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="B104" t="s">
         <v>43</v>
@@ -1608,7 +1967,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>39</v>
+        <v>159</v>
       </c>
       <c r="B105" t="s">
         <v>43</v>
@@ -1616,15 +1975,15 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>40</v>
+        <v>160</v>
       </c>
       <c r="B106" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>41</v>
+        <v>161</v>
       </c>
       <c r="B107" t="s">
         <v>44</v>
@@ -1632,7 +1991,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B108" t="s">
         <v>44</v>
@@ -1640,15 +1999,15 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>43</v>
+        <v>163</v>
       </c>
       <c r="B109" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>44</v>
+        <v>164</v>
       </c>
       <c r="B110" t="s">
         <v>45</v>
@@ -1656,15 +2015,15 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>31</v>
+        <v>165</v>
       </c>
       <c r="B111" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>36</v>
+        <v>166</v>
       </c>
       <c r="B112" t="s">
         <v>46</v>
@@ -1672,15 +2031,15 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>106</v>
+        <v>167</v>
       </c>
       <c r="B113" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>107</v>
+        <v>168</v>
       </c>
       <c r="B114" t="s">
         <v>47</v>
@@ -1688,15 +2047,15 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>108</v>
+        <v>169</v>
       </c>
       <c r="B115" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>106</v>
+        <v>170</v>
       </c>
       <c r="B116" t="s">
         <v>48</v>
@@ -1704,15 +2063,15 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>109</v>
+        <v>171</v>
       </c>
       <c r="B117" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>110</v>
+        <v>172</v>
       </c>
       <c r="B118" t="s">
         <v>49</v>
@@ -1720,7 +2079,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>111</v>
+        <v>173</v>
       </c>
       <c r="B119" t="s">
         <v>49</v>
@@ -1728,15 +2087,15 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>112</v>
+        <v>174</v>
       </c>
       <c r="B120" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>106</v>
+        <v>175</v>
       </c>
       <c r="B121" t="s">
         <v>50</v>
@@ -1744,15 +2103,15 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>113</v>
+        <v>176</v>
       </c>
       <c r="B122" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>114</v>
+        <v>177</v>
       </c>
       <c r="B123" t="s">
         <v>51</v>
@@ -1760,7 +2119,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>106</v>
+        <v>178</v>
       </c>
       <c r="B124" t="s">
         <v>51</v>
@@ -1768,15 +2127,15 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>47</v>
+        <v>179</v>
       </c>
       <c r="B125" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>48</v>
+        <v>180</v>
       </c>
       <c r="B126" t="s">
         <v>52</v>
@@ -1784,15 +2143,15 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>49</v>
+        <v>181</v>
       </c>
       <c r="B127" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>50</v>
+        <v>182</v>
       </c>
       <c r="B128" t="s">
         <v>53</v>
@@ -1800,7 +2159,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>51</v>
+        <v>183</v>
       </c>
       <c r="B129" t="s">
         <v>53</v>
@@ -1808,15 +2167,15 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>52</v>
+        <v>184</v>
       </c>
       <c r="B130" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>53</v>
+        <v>185</v>
       </c>
       <c r="B131" t="s">
         <v>54</v>
@@ -1824,15 +2183,15 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>8</v>
+        <v>186</v>
       </c>
       <c r="B132" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>27</v>
+        <v>187</v>
       </c>
       <c r="B133" t="s">
         <v>55</v>
@@ -1840,7 +2199,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="B134" t="s">
         <v>55</v>
@@ -1848,7 +2207,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>35</v>
+        <v>189</v>
       </c>
       <c r="B135" t="s">
         <v>55</v>
@@ -1856,15 +2215,15 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>115</v>
+        <v>190</v>
       </c>
       <c r="B136" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="B137" t="s">
         <v>56</v>
@@ -1872,7 +2231,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>54</v>
+        <v>191</v>
       </c>
       <c r="B138" t="s">
         <v>56</v>
@@ -1880,9 +2239,17 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>116</v>
+        <v>192</v>
       </c>
       <c r="B139" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>61</v>
+      </c>
+      <c r="B140" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
After fixing the basic leve indicator changes
</commit_message>
<xml_diff>
--- a/Node_relationship.xlsx
+++ b/Node_relationship.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nandhu\comeai\Result_Share\Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B83C25-6C1F-4384-9647-54BDBF02C7C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF5E6D7-3633-489E-82C4-269F5244964B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{87162CFC-B4E0-45F1-A01A-41825A97D9AF}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$139</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$140</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1122,10 +1122,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A99ED6B7-327B-491C-9CB5-D727B291EEBF}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:B140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1141,7 +1142,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -1149,7 +1150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -1157,7 +1158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -1165,7 +1166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -1173,7 +1174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -1181,7 +1182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -1189,7 +1190,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>68</v>
       </c>
@@ -1197,7 +1198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -1205,7 +1206,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -1213,7 +1214,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>71</v>
       </c>
@@ -1221,7 +1222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -1229,7 +1230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -1237,7 +1238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -1245,7 +1246,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -1253,7 +1254,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -1261,7 +1262,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -1269,7 +1270,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -1277,7 +1278,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -1285,7 +1286,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -1293,7 +1294,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -1301,7 +1302,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>82</v>
       </c>
@@ -1309,7 +1310,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>83</v>
       </c>
@@ -1317,7 +1318,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -1325,7 +1326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>85</v>
       </c>
@@ -1333,7 +1334,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>86</v>
       </c>
@@ -1341,7 +1342,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>87</v>
       </c>
@@ -1349,7 +1350,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -1357,7 +1358,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>89</v>
       </c>
@@ -1365,7 +1366,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>90</v>
       </c>
@@ -1373,7 +1374,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>91</v>
       </c>
@@ -1381,7 +1382,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>92</v>
       </c>
@@ -1389,7 +1390,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>93</v>
       </c>
@@ -1397,7 +1398,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>94</v>
       </c>
@@ -1405,7 +1406,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>95</v>
       </c>
@@ -1413,7 +1414,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>96</v>
       </c>
@@ -1421,7 +1422,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>97</v>
       </c>
@@ -1429,7 +1430,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>98</v>
       </c>
@@ -1437,7 +1438,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>96</v>
       </c>
@@ -1445,7 +1446,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>99</v>
       </c>
@@ -1453,7 +1454,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>100</v>
       </c>
@@ -1461,7 +1462,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>101</v>
       </c>
@@ -1469,7 +1470,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>102</v>
       </c>
@@ -1477,7 +1478,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>103</v>
       </c>
@@ -1485,7 +1486,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>104</v>
       </c>
@@ -1493,7 +1494,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>105</v>
       </c>
@@ -1501,7 +1502,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>106</v>
       </c>
@@ -1509,7 +1510,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>107</v>
       </c>
@@ -1517,7 +1518,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>108</v>
       </c>
@@ -1525,7 +1526,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>109</v>
       </c>
@@ -1533,7 +1534,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>110</v>
       </c>
@@ -1541,7 +1542,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>111</v>
       </c>
@@ -1549,7 +1550,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>112</v>
       </c>
@@ -1557,7 +1558,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>113</v>
       </c>
@@ -1565,7 +1566,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>114</v>
       </c>
@@ -1573,7 +1574,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>115</v>
       </c>
@@ -1581,7 +1582,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>116</v>
       </c>
@@ -1589,7 +1590,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>117</v>
       </c>
@@ -1597,7 +1598,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>118</v>
       </c>
@@ -1605,7 +1606,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>119</v>
       </c>
@@ -1613,7 +1614,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>120</v>
       </c>
@@ -1621,7 +1622,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>121</v>
       </c>
@@ -1629,7 +1630,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>122</v>
       </c>
@@ -1637,7 +1638,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>123</v>
       </c>
@@ -1645,7 +1646,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>124</v>
       </c>
@@ -1653,7 +1654,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>125</v>
       </c>
@@ -1661,7 +1662,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>126</v>
       </c>
@@ -1669,7 +1670,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>127</v>
       </c>
@@ -1677,7 +1678,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>128</v>
       </c>
@@ -1685,7 +1686,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>129</v>
       </c>
@@ -1693,7 +1694,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>130</v>
       </c>
@@ -1701,7 +1702,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>131</v>
       </c>
@@ -1709,7 +1710,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>132</v>
       </c>
@@ -1717,7 +1718,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>133</v>
       </c>
@@ -1725,7 +1726,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>134</v>
       </c>
@@ -1733,7 +1734,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>135</v>
       </c>
@@ -1741,7 +1742,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>136</v>
       </c>
@@ -1749,7 +1750,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>137</v>
       </c>
@@ -1757,7 +1758,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>138</v>
       </c>
@@ -1765,7 +1766,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>139</v>
       </c>
@@ -1773,7 +1774,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>131</v>
       </c>
@@ -1781,7 +1782,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>140</v>
       </c>
@@ -1789,7 +1790,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>141</v>
       </c>
@@ -1797,7 +1798,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>142</v>
       </c>
@@ -1805,7 +1806,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>143</v>
       </c>
@@ -1813,7 +1814,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>144</v>
       </c>
@@ -1821,7 +1822,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>145</v>
       </c>
@@ -1829,7 +1830,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>146</v>
       </c>
@@ -1837,7 +1838,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>147</v>
       </c>
@@ -1845,7 +1846,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>148</v>
       </c>
@@ -1877,7 +1878,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>150</v>
       </c>
@@ -1885,7 +1886,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>147</v>
       </c>
@@ -1893,7 +1894,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>148</v>
       </c>
@@ -1901,7 +1902,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>151</v>
       </c>
@@ -1909,7 +1910,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>152</v>
       </c>
@@ -1917,7 +1918,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>153</v>
       </c>
@@ -1925,7 +1926,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>154</v>
       </c>
@@ -1933,7 +1934,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>155</v>
       </c>
@@ -1941,7 +1942,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>156</v>
       </c>
@@ -1949,7 +1950,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>157</v>
       </c>
@@ -1957,7 +1958,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>158</v>
       </c>
@@ -1965,7 +1966,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>159</v>
       </c>
@@ -1973,7 +1974,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>160</v>
       </c>
@@ -1981,7 +1982,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>161</v>
       </c>
@@ -1989,7 +1990,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>162</v>
       </c>
@@ -1997,7 +1998,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>163</v>
       </c>
@@ -2005,7 +2006,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>164</v>
       </c>
@@ -2013,7 +2014,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>165</v>
       </c>
@@ -2021,7 +2022,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>166</v>
       </c>
@@ -2029,7 +2030,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>167</v>
       </c>
@@ -2037,7 +2038,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>168</v>
       </c>
@@ -2045,7 +2046,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>169</v>
       </c>
@@ -2053,7 +2054,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>170</v>
       </c>
@@ -2061,7 +2062,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>171</v>
       </c>
@@ -2069,7 +2070,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>172</v>
       </c>
@@ -2077,7 +2078,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>173</v>
       </c>
@@ -2085,7 +2086,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>174</v>
       </c>
@@ -2093,7 +2094,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>175</v>
       </c>
@@ -2101,7 +2102,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>176</v>
       </c>
@@ -2109,7 +2110,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>177</v>
       </c>
@@ -2117,7 +2118,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>178</v>
       </c>
@@ -2125,7 +2126,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>179</v>
       </c>
@@ -2133,7 +2134,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>180</v>
       </c>
@@ -2141,7 +2142,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>181</v>
       </c>
@@ -2149,7 +2150,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>182</v>
       </c>
@@ -2157,7 +2158,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>183</v>
       </c>
@@ -2165,7 +2166,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>184</v>
       </c>
@@ -2173,7 +2174,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>185</v>
       </c>
@@ -2181,7 +2182,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>186</v>
       </c>
@@ -2189,7 +2190,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>187</v>
       </c>
@@ -2197,7 +2198,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>188</v>
       </c>
@@ -2205,7 +2206,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>189</v>
       </c>
@@ -2213,7 +2214,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>190</v>
       </c>
@@ -2221,7 +2222,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>60</v>
       </c>
@@ -2229,7 +2230,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>191</v>
       </c>
@@ -2237,7 +2238,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>192</v>
       </c>
@@ -2245,7 +2246,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>61</v>
       </c>
@@ -2254,6 +2255,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:B140" xr:uid="{A99ED6B7-327B-491C-9CB5-D727B291EEBF}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="C2_2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>